<commit_message>
Action & Password Updation
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>PRN</t>
   </si>
@@ -26,6 +26,30 @@
   </si>
   <si>
     <t>Marks</t>
+  </si>
+  <si>
+    <t>2020078384</t>
+  </si>
+  <si>
+    <t>2022208485</t>
+  </si>
+  <si>
+    <t>PrathmeshSutar</t>
+  </si>
+  <si>
+    <t>Sangram Kamable</t>
+  </si>
+  <si>
+    <t>dyp</t>
+  </si>
+  <si>
+    <t>DKTE</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>85</t>
   </si>
 </sst>
 </file>
@@ -383,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,6 +427,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>